<commit_message>
terminando o robo performer
</commit_message>
<xml_diff>
--- a/Performer/Data/Config.xlsx
+++ b/Performer/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CATALOG\Documents\UiPath\RPA_UdemyMarceloCruz\Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CATALOG\Documents\UiPath\RPA_UdemyMarceloCruz\Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABA1DCB-1235-4D91-9AEB-5F1E2F1659FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE97ED1-E611-468D-A310-16883E1AF5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,16 +167,16 @@
     <t>ACME_Credenciais</t>
   </si>
   <si>
-    <t>ACME_VisualizarFaturas_URL</t>
-  </si>
-  <si>
-    <t>https://acme-test.uipath.com/invoices/search-by-vendor</t>
-  </si>
-  <si>
     <t>OrchestratorNomeFila</t>
   </si>
   <si>
     <t>FilaFaturas</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/invoices/search</t>
+  </si>
+  <si>
+    <t>ACME_ProcurarFatura_URL</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -619,10 +619,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -669,10 +669,10 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6"/>
     </row>

</xml_diff>